<commit_message>
Se añadieron nuevos temas al archivo turismo y se ajustaron los archivos html
</commit_message>
<xml_diff>
--- a/myapp/files/log.xlsx
+++ b/myapp/files/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -456,8 +456,10 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>102</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
@@ -466,7 +468,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Hi there, what can I do for you?</t>
+          <t>¡Bienvenido/a al Quindío! Soy Kofi, el chatbot con el calor de nuestras montañas y la pasión de nuestra gente. ¿Qué te gustaría saber sobre nuestra tierra cafetera y cómo puedo hacer tu visita más memorable?</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -476,37 +478,41 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>102</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>deporte</t>
+          <t>deseo almorzar</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>El Valle del Cócora: Este es un lugar perfecto para hacer canopy y tirolesa, donde puedes disfrutar de las vistas de los paisajes montañosos y los valles verdes.</t>
+          <t>¡Claro, mi amigo! Si quieres degustar los sabores tradicionales de nuestra región, te recomiendo el restaurante 'La Cocina de la Abuela', en Salento. Allí podrás disfrutar de platos como el ají de pollo y el famoso tamal quindiano. Además, el ambiente rústico y acogedor te hará sentir como parte de nuestra familia quindiana.</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>deportes_extremos</t>
+          <t>restaurantes</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>102</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>recomiendame un lugar a visitar</t>
+          <t>quiero explorar el quindio</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Te recomiendo ir a Quimbaya</t>
+          <t>¡Así es, mi amigo explorador! Quimbaya es un destino que te sorprenderá con su autenticidad y su riqueza cultural. Y si eres amante de la naturaleza, te invito a explorar el Parque Nacional Natural Los Nevados, un lugar que te ofrece paisajes impresionantes y la oportunidad de estar en contacto con la flora y fauna de nuestra región.</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
@@ -516,17 +522,19 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>102</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t xml:space="preserve">tengo hambre quiero almorzar </t>
+          <t>adios</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Te sugiero el restaurante Container</t>
+          <t>¡Hola, mi estimado visitante! Si estás en Quimbaya, te recomiendo el restaurante 'El Rancherito'. Allí podrás disfrutar de la auténtica comida quindiana, como el famoso ajiaco y el suculento lechón asado. Además, el ambiente familiar y cálido te hará sentir como en casa, rodeado de nuestras hermosas montañas.</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
@@ -536,17 +544,19 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>102</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>hi</t>
+          <t>hola</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Hello, how can I assist you today?</t>
+          <t>¡Bienvenido/a a Kofi, tu guía virtual del Quindío! ¿Tienes curiosidad por conocer nuestros paisajes exuberantes, nuestra cultura cafetera o nuestras actividades emocionantes? Estoy aquí para ayudarte.</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
@@ -556,184 +566,68 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>102</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>quiero visitar algun lugar</t>
+          <t>tienes museos</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Te recomiendo ir a Quimbaya</t>
+          <t>¡Amigo turista, estás en el lugar indicado para saborear lo mejor del Quindío! Te sugiero visitar el restaurante 'El Fogón de Doña Rosa' en Filandia. Allí encontrarás delicias como el mondongo quindiano y las empanadas de pipián. Es un lugar donde la tradición y la buena comida se fusionan en cada plato. ¡No te lo puedes perder!</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>sitios</t>
+          <t>restaurantes</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr"/>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>hola</t>
+          <t>deseo desayunar</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Circasia: Este es un pueblo ubicado en el centro del QuindÃ­o, que ofrece opciones para hacer ciclismo de montaÃ±a y senderismo.</t>
+          <t>¡Bienvenido a nuestro paraíso gastronómico, mi amigo! Si buscas una experiencia culinaria única, te sugiero el restaurante 'El Mirador' en el Parque Nacional Natural Los Nevados. Podrás degustar platos gourmet con ingredientes frescos y locales, mientras disfrutas de las impresionantes vistas de nuestros paisajes montañosos. ¡Será una experiencia inolvidable para tus sentidos!</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>deportes_extremos</t>
+          <t>restaurantes</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr"/>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>123456789</t>
+        </is>
+      </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>hola como estas</t>
+          <t>chao</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>El Valle del CÃ³cora: Este es un lugar perfecto para hacer canopy y tirolesa, donde puedes disfrutar de las vistas de los paisajes montaÃ±osos y los valles verdes.</t>
+          <t>¡Por supuesto, mi estimado visitante! Te sugiero probar el restaurante 'Sabor Quindiano'. Ahí encontrarás los sabores auténticos de nuestra tierra, como el inigualable sancocho de gallina y las arepas de chócolo. Está ubicado en el centro de Armenia, en la Calle 14, justo al lado de la Plaza de Bolívar. Te sentirás como en casa, disfrutando de nuestra deliciosa gastronomía.</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr"/>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Parque del CafÃ©: Este parque temÃ¡tico ofrece varias atracciones emocionantes, incluyendo montaÃ±as rusas y atracciones acuÃ¡ticas.</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr"/>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Circasia: Este es un pueblo ubicado en el centro del QuindÃ­o, que ofrece opciones para hacer ciclismo de montaÃ±a y senderismo.</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr"/>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Salento: Este es un pueblo pintoresco ubicado en el Valle de Cocora, que ofrece varias opciones para hacer senderismo y caminatas extremas.</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr"/>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Parque Nacional Natural Los Nevados: Este parque es un lugar ideal para hacer senderismo y montaÃ±ismo. AquÃ­ puedes encontrar varios picos altos y rutas desafiantes.</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr"/>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>hola</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Salento: Este es un pueblo pintoresco ubicado en el Valle de Cocora, que ofrece varias opciones para hacer senderismo y caminatas extremas.</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>deportes_extremos</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr"/>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>almorzar</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Hello, how can I help you?</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>saludo</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr"/>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>quiero un sitio para comer</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Te recomiendo visitar Casa Museo Pueblito Cafetero</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>museos</t>
+          <t>restaurantes</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Se modifico la interfaz del chatbot
</commit_message>
<xml_diff>
--- a/myapp/files/log.xlsx
+++ b/myapp/files/log.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1376,24 +1376,88 @@
       </c>
     </row>
     <row r="48">
-      <c r="A48" t="inlineStr">
+      <c r="A48" t="n">
+        <v>1005897049</v>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>deportes extremos</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Salento: Este es un pueblo pintoresco ubicado en el Valle de Cocora, que ofrece varias opciones para hacer senderismo y caminatas extremas.</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>deportes_extremos</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
         <is>
           <t>1005897049</t>
         </is>
       </c>
-      <c r="B48" t="inlineStr">
+      <c r="B49" t="inlineStr">
         <is>
           <t>deportes extremos</t>
         </is>
       </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Salento: Este es un pueblo pintoresco ubicado en el Valle de Cocora, que ofrece varias opciones para hacer senderismo y caminatas extremas.</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Circasia: Este es un pueblo ubicado en el centro del Quindío, que ofrece opciones para hacer ciclismo de montaña y senderismo.</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
         <is>
           <t>deportes_extremos</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>quiero comer algo para almorzar</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>¡Bienvenido a nuestro paraíso gastronómico, mi amigo! Si buscas una experiencia culinaria única, te sugiero el restaurante 'El Mirador' en el Parque Nacional Natural Los Nevados. Podrás degustar platos gourmet con ingredientes frescos y locales, mientras disfrutas de las impresionantes vistas de nuestros paisajes montañosos. ¡Será una experiencia inolvidable para tus sentidos!</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>restaurantes</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>1005897049</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>dame un buen museo para ir con la familia</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>¡Claro que sí! En el Quindío, contamos con una amplia variedad de opciones de alojamiento para todos los gustos y presupuestos. Podría recomendarte el Hotel Campestre La Finca, un lugar acogedor rodeado de naturaleza donde podrás disfrutar de la tranquilidad y comodidad. También puedes considerar la Posada El Mirador, con vistas panorámicas increíbles de nuestros paisajes.</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>alojamiento</t>
         </is>
       </c>
     </row>

</xml_diff>